<commit_message>
test for drop NA
</commit_message>
<xml_diff>
--- a/test_data_1.xlsx
+++ b/test_data_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://areasciencepark-my.sharepoint.com/personal/fabio_morea_areasciencepark_it/Documents/Documents/2022/CodiciGreen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{138E807E-7713-4969-8332-3DC37D47EF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4C77E01-A5B7-437E-8170-7CDB8FE2BD7F}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{138E807E-7713-4969-8332-3DC37D47EF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7725AB0B-30F1-45FD-AA3B-42EAC606B737}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{890FC4FF-8082-4EC9-9E49-B0766CB45614}"/>
   </bookViews>
@@ -99,12 +99,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -117,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -435,7 +444,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>